<commit_message>
Begin conversion from spreadsheets
</commit_message>
<xml_diff>
--- a/background/eLTSS to FHIR R4 element mapping_2019-01-24.xlsx
+++ b/background/eLTSS to FHIR R4 element mapping_2019-01-24.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{36C24330-0952-4B8A-8895-63B2735108B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{E624EAE6-A34B-49ED-8254-16B077AA2C3D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EA1B68-977B-4DEB-BA3C-B4DBDF8859DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="108" windowWidth="28296" windowHeight="13992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eLTSS element mapping" sheetId="2" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="683">
   <si>
     <t>Data Element Definition</t>
   </si>
@@ -34408,26 +34408,26 @@
   </sheetPr>
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="47.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" customWidth="1"/>
     <col min="6" max="6" width="40" customWidth="1"/>
-    <col min="7" max="7" width="40.109375" customWidth="1"/>
-    <col min="8" max="8" width="45.44140625" customWidth="1"/>
-    <col min="9" max="9" width="68.33203125" customWidth="1"/>
-    <col min="10" max="10" width="31.88671875" customWidth="1"/>
+    <col min="7" max="7" width="40.140625" customWidth="1"/>
+    <col min="8" max="8" width="45.42578125" customWidth="1"/>
+    <col min="9" max="9" width="68.28515625" customWidth="1"/>
+    <col min="10" max="10" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>483</v>
       </c>
@@ -34459,7 +34459,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>68</v>
       </c>
@@ -34491,7 +34491,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>68</v>
       </c>
@@ -34523,7 +34523,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
@@ -34555,7 +34555,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>68</v>
       </c>
@@ -34587,7 +34587,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>68</v>
       </c>
@@ -34619,7 +34619,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>68</v>
       </c>
@@ -34651,7 +34651,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>68</v>
       </c>
@@ -34683,7 +34683,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="203.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="203.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>68</v>
       </c>
@@ -34715,7 +34715,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>68</v>
       </c>
@@ -34747,7 +34747,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="318" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="318" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>68</v>
       </c>
@@ -34779,7 +34779,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -34811,7 +34811,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="309" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="309" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>81</v>
       </c>
@@ -34843,7 +34843,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>81</v>
       </c>
@@ -34875,7 +34875,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="319.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="319.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>82</v>
       </c>
@@ -34907,7 +34907,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>82</v>
       </c>
@@ -34939,7 +34939,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>82</v>
       </c>
@@ -34971,7 +34971,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
@@ -35003,7 +35003,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>82</v>
       </c>
@@ -35035,7 +35035,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>82</v>
       </c>
@@ -35067,7 +35067,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>82</v>
       </c>
@@ -35099,7 +35099,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>82</v>
       </c>
@@ -35131,7 +35131,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>82</v>
       </c>
@@ -35163,7 +35163,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
@@ -35195,7 +35195,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>82</v>
       </c>
@@ -35227,7 +35227,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>86</v>
       </c>
@@ -35259,7 +35259,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="245.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
@@ -35291,7 +35291,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>89</v>
       </c>
@@ -35323,7 +35323,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>89</v>
       </c>
@@ -35355,7 +35355,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="348.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="348.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
@@ -35387,7 +35387,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="146.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="146.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>89</v>
       </c>
@@ -35419,7 +35419,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>89</v>
       </c>
@@ -35451,7 +35451,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="342" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="342" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>89</v>
       </c>
@@ -35483,7 +35483,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="144.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="144.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>89</v>
       </c>
@@ -35515,7 +35515,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>89</v>
       </c>
@@ -35547,7 +35547,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="346.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="346.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>89</v>
       </c>
@@ -35579,7 +35579,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="173.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>89</v>
       </c>
@@ -35611,7 +35611,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>89</v>
       </c>
@@ -35643,7 +35643,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>105</v>
       </c>
@@ -35675,7 +35675,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="303" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="303" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>105</v>
       </c>
@@ -35707,7 +35707,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>107</v>
       </c>
@@ -35739,7 +35739,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>107</v>
       </c>
@@ -35771,7 +35771,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>107</v>
       </c>
@@ -35803,7 +35803,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>107</v>
       </c>
@@ -35835,7 +35835,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="173.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>107</v>
       </c>
@@ -35867,7 +35867,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>107</v>
       </c>
@@ -35899,7 +35899,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="196.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="196.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>107</v>
       </c>
@@ -35931,7 +35931,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>107</v>
       </c>
@@ -35963,7 +35963,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="216.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>107</v>
       </c>
@@ -35995,7 +35995,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>107</v>
       </c>
@@ -36027,7 +36027,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="273" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="273" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>107</v>
       </c>
@@ -36059,7 +36059,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>107</v>
       </c>
@@ -36091,7 +36091,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>114</v>
       </c>
@@ -36123,7 +36123,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>114</v>
       </c>
@@ -36155,7 +36155,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="177.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="177.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>114</v>
       </c>
@@ -36187,7 +36187,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="245.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>114</v>
       </c>
@@ -36219,7 +36219,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="165.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="165.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>114</v>
       </c>
@@ -36269,22 +36269,22 @@
   </sheetPr>
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="47.44140625" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="40.109375" customWidth="1"/>
-    <col min="6" max="6" width="68.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="57" t="s">
         <v>505</v>
       </c>
@@ -36294,7 +36294,7 @@
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
     </row>
-    <row r="2" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>488</v>
       </c>
@@ -36314,7 +36314,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>450</v>
       </c>
@@ -36334,7 +36334,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>451</v>
       </c>
@@ -36354,7 +36354,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>452</v>
       </c>
@@ -36374,7 +36374,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>453</v>
       </c>
@@ -36394,7 +36394,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>454</v>
       </c>
@@ -36414,7 +36414,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>455</v>
       </c>
@@ -36434,7 +36434,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>456</v>
       </c>
@@ -36454,7 +36454,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>457</v>
       </c>
@@ -36474,7 +36474,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>458</v>
       </c>
@@ -36494,7 +36494,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="51" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" s="51" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="53" t="s">
         <v>595</v>
       </c>
@@ -36514,7 +36514,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="51" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" s="51" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="53" t="s">
         <v>618</v>
       </c>
@@ -36534,7 +36534,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="51" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" s="51" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="53" t="s">
         <v>622</v>
       </c>
@@ -36554,7 +36554,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="51" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" s="51" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
         <v>623</v>
       </c>
@@ -36574,7 +36574,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="51" customFormat="1" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" s="51" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="53" t="s">
         <v>624</v>
       </c>
@@ -36594,7 +36594,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="51" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" s="51" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="53" t="s">
         <v>637</v>
       </c>
@@ -36614,7 +36614,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="51" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" s="51" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="53" t="s">
         <v>590</v>
       </c>
@@ -36634,7 +36634,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="51" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" s="51" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="53" t="s">
         <v>612</v>
       </c>
@@ -36654,7 +36654,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="51" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" s="51" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="53" t="s">
         <v>606</v>
       </c>
@@ -36674,7 +36674,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="51" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" s="51" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="53" t="s">
         <v>567</v>
       </c>
@@ -36694,7 +36694,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="51" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" s="51" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="53" t="s">
         <v>581</v>
       </c>
@@ -36714,7 +36714,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="51" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" s="51" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="53" t="s">
         <v>586</v>
       </c>
@@ -36734,7 +36734,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>459</v>
       </c>
@@ -36754,7 +36754,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>460</v>
       </c>
@@ -36774,7 +36774,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>461</v>
       </c>
@@ -36794,7 +36794,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>462</v>
       </c>
@@ -36814,7 +36814,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="51" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" s="51" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="53" t="s">
         <v>577</v>
       </c>
@@ -36834,7 +36834,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="51" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" s="51" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="53" t="s">
         <v>578</v>
       </c>
@@ -36854,7 +36854,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="51" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" s="51" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="53" t="s">
         <v>642</v>
       </c>
@@ -36874,7 +36874,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>463</v>
       </c>
@@ -36894,7 +36894,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="53" t="s">
         <v>679</v>
       </c>
@@ -36914,7 +36914,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="53" t="s">
         <v>681</v>
       </c>
@@ -36934,7 +36934,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
         <v>464</v>
       </c>
@@ -36954,7 +36954,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
         <v>465</v>
       </c>
@@ -36974,7 +36974,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="54" t="s">
         <v>554</v>
       </c>
@@ -36994,7 +36994,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="22" t="s">
         <v>466</v>
       </c>
@@ -37014,7 +37014,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22" t="s">
         <v>467</v>
       </c>
@@ -37034,7 +37034,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>468</v>
       </c>
@@ -37054,7 +37054,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="22" t="s">
         <v>469</v>
       </c>
@@ -37074,7 +37074,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22" t="s">
         <v>470</v>
       </c>
@@ -37094,7 +37094,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="22" t="s">
         <v>471</v>
       </c>
@@ -37114,7 +37114,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="22" t="s">
         <v>472</v>
       </c>
@@ -37134,7 +37134,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="22" t="s">
         <v>473</v>
       </c>
@@ -37154,7 +37154,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="22" t="s">
         <v>474</v>
       </c>
@@ -37174,7 +37174,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
         <v>475</v>
       </c>
@@ -37194,7 +37194,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="22" t="s">
         <v>476</v>
       </c>
@@ -37214,7 +37214,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="22" t="s">
         <v>477</v>
       </c>
@@ -37234,7 +37234,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="22" t="s">
         <v>478</v>
       </c>
@@ -37254,7 +37254,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="22" t="s">
         <v>479</v>
       </c>
@@ -37274,7 +37274,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22" t="s">
         <v>480</v>
       </c>
@@ -37294,7 +37294,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22" t="s">
         <v>481</v>
       </c>
@@ -37314,7 +37314,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="22" t="s">
         <v>482</v>
       </c>
@@ -37355,26 +37355,26 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" style="10" customWidth="1"/>
-    <col min="2" max="2" width="97.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="6"/>
-    <col min="5" max="5" width="29.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="56.44140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="6"/>
-    <col min="8" max="8" width="29.6640625" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="6"/>
+    <col min="2" max="2" width="97.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="71.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="6"/>
+    <col min="5" max="5" width="29.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="56.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="6"/>
+    <col min="8" max="8" width="29.7109375" style="6" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="58" t="s">
         <v>484</v>
       </c>
       <c r="B1" s="59"/>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>147</v>
       </c>
@@ -37382,7 +37382,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>483</v>
       </c>
@@ -37391,7 +37391,7 @@
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>485</v>
       </c>
@@ -37400,7 +37400,7 @@
       </c>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:3" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
         <v>490</v>
       </c>
@@ -37409,7 +37409,7 @@
       </c>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:3" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
@@ -37418,7 +37418,7 @@
       </c>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>489</v>
       </c>
@@ -37427,7 +37427,7 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" ht="145.19999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>417</v>
       </c>
@@ -37436,7 +37436,7 @@
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" ht="116.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="151.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="47" t="s">
         <v>419</v>
       </c>
@@ -37445,7 +37445,7 @@
       </c>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>58</v>
       </c>
@@ -37454,7 +37454,7 @@
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>149</v>
       </c>
@@ -37463,7 +37463,7 @@
       </c>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" ht="300.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="300.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>131</v>
       </c>
@@ -37472,7 +37472,7 @@
       </c>
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:3" ht="13.8" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" ht="13.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
@@ -37498,21 +37498,21 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="39" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="39" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="39" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="39" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="39" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="39" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>340</v>
       </c>
@@ -37532,7 +37532,7 @@
       <c r="I1" s="62"/>
       <c r="J1" s="62"/>
     </row>
-    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="60"/>
       <c r="B2" s="28" t="s">
         <v>341</v>
@@ -37562,7 +37562,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>344</v>
       </c>
@@ -37590,7 +37590,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>347</v>
       </c>
@@ -37618,7 +37618,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>350</v>
       </c>
@@ -37646,7 +37646,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>352</v>
       </c>
@@ -37674,7 +37674,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>354</v>
       </c>
@@ -37702,7 +37702,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
         <v>358</v>
       </c>
@@ -37730,7 +37730,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
         <v>359</v>
       </c>
@@ -37758,7 +37758,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
         <v>361</v>
       </c>
@@ -37782,7 +37782,7 @@
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>362</v>
       </c>
@@ -37810,7 +37810,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
         <v>364</v>
       </c>
@@ -37834,7 +37834,7 @@
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>365</v>
       </c>
@@ -37856,7 +37856,7 @@
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>368</v>
       </c>
@@ -37880,7 +37880,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>370</v>
       </c>
@@ -37904,7 +37904,7 @@
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>372</v>
       </c>
@@ -37932,7 +37932,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>373</v>
       </c>
@@ -37960,7 +37960,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
         <v>533</v>
       </c>
@@ -37988,7 +37988,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>510</v>
       </c>
@@ -37999,7 +37999,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C21" s="35" t="s">
         <v>375</v>
       </c>
@@ -38007,7 +38007,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C22" s="35" t="s">
         <v>355</v>
       </c>
@@ -38015,7 +38015,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C23" s="35" t="s">
         <v>345</v>
       </c>
@@ -38023,7 +38023,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="35" t="s">
         <v>351</v>
       </c>
@@ -38031,7 +38031,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C25" s="35" t="s">
         <v>348</v>
       </c>
@@ -38039,27 +38039,27 @@
         <v>378</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C26" s="35" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="35" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" s="35" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C29" s="35" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="C30" s="35" t="s">
         <v>363</v>
@@ -38072,7 +38072,7 @@
       <c r="J30"/>
       <c r="K30"/>
     </row>
-    <row r="31" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="C31" s="35" t="s">
         <v>374</v>
@@ -38085,7 +38085,7 @@
       <c r="J31"/>
       <c r="K31"/>
     </row>
-    <row r="32" spans="1:11" s="39" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" s="39" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="C32" s="41" t="s">
         <v>382</v>
@@ -38098,7 +38098,7 @@
       <c r="J32"/>
       <c r="K32"/>
     </row>
-    <row r="33" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="C33" s="35" t="s">
         <v>369</v>
@@ -38111,7 +38111,7 @@
       <c r="J33"/>
       <c r="K33"/>
     </row>
-    <row r="34" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="C34" s="35" t="s">
         <v>366</v>
@@ -38124,7 +38124,7 @@
       <c r="J34"/>
       <c r="K34"/>
     </row>
-    <row r="35" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="C35" s="35" t="s">
         <v>383</v>

</xml_diff>